<commit_message>
test commit from dell 6/23-1
</commit_message>
<xml_diff>
--- a/case.xlsx
+++ b/case.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="115">
   <si>
     <t>编号</t>
   </si>
@@ -370,6 +370,9 @@
   </si>
   <si>
     <t>通过webhook.create去创建一个webhookurl</t>
+  </si>
+  <si>
+    <t>修改dell</t>
   </si>
 </sst>
 </file>
@@ -1710,8 +1713,8 @@
   <sheetPr/>
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14"/>
@@ -2521,12 +2524,15 @@
       <c r="B33" s="10"/>
       <c r="C33" s="4"/>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:4">
       <c r="A34" s="4">
         <v>31</v>
       </c>
       <c r="B34" s="10"/>
       <c r="C34" s="4"/>
+      <c r="D34" s="4" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="4">

</xml_diff>

<commit_message>
commit from arikan-dell 250625-1
</commit_message>
<xml_diff>
--- a/case.xlsx
+++ b/case.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25600" windowHeight="12790"/>
+    <workbookView windowWidth="24750" windowHeight="12790"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="126">
   <si>
     <t>编号</t>
   </si>
@@ -35,22 +35,22 @@
     <t>时间</t>
   </si>
   <si>
-    <t>status</t>
+    <t>状态</t>
+  </si>
+  <si>
+    <t>问题来源</t>
+  </si>
+  <si>
+    <t>问题描述</t>
+  </si>
+  <si>
+    <t>问题原因</t>
+  </si>
+  <si>
+    <t>解决方案</t>
   </si>
   <si>
     <t>问题提出时间</t>
-  </si>
-  <si>
-    <t>问题来源</t>
-  </si>
-  <si>
-    <t>问题描述</t>
-  </si>
-  <si>
-    <t>问题原因</t>
-  </si>
-  <si>
-    <t>解决方案</t>
   </si>
   <si>
     <t>方案提出时间</t>
@@ -403,6 +403,9 @@
   </si>
   <si>
     <t>东海排查中</t>
+  </si>
+  <si>
+    <t>6、26修改</t>
   </si>
 </sst>
 </file>
@@ -1115,7 +1118,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1131,6 +1134,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -1152,15 +1158,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1173,9 +1179,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="fill" vertical="center" wrapText="1"/>
     </xf>
@@ -1185,6 +1188,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1203,8 +1209,14 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1741,25 +1753,25 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K48"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:A48"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="5" style="4" customWidth="1"/>
     <col min="2" max="2" width="5" customWidth="1"/>
-    <col min="3" max="3" width="6.36363636363636" customWidth="1"/>
-    <col min="4" max="4" width="17.9090909090909" style="4" customWidth="1"/>
-    <col min="5" max="5" width="15.4545454545455" style="4" customWidth="1"/>
-    <col min="6" max="6" width="41.4545454545455" style="5" customWidth="1"/>
-    <col min="7" max="7" width="34.3636363636364" style="6" customWidth="1"/>
-    <col min="8" max="8" width="48.9090909090909" style="7" customWidth="1"/>
+    <col min="3" max="3" width="4.54545454545455" customWidth="1"/>
+    <col min="4" max="4" width="15.4545454545455" style="5" customWidth="1"/>
+    <col min="5" max="5" width="41.4545454545455" style="6" customWidth="1"/>
+    <col min="6" max="6" width="34.3636363636364" style="7" customWidth="1"/>
+    <col min="7" max="7" width="48.9090909090909" style="8" customWidth="1"/>
+    <col min="8" max="8" width="17.9090909090909" style="4" customWidth="1"/>
     <col min="9" max="9" width="17.7272727272727" style="4" customWidth="1"/>
     <col min="10" max="10" width="22.2727272727273" style="4" customWidth="1"/>
-    <col min="11" max="11" width="43.2727272727273" style="8" customWidth="1"/>
+    <col min="11" max="11" width="43.2727272727273" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:11">
@@ -1775,16 +1787,16 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -1801,29 +1813,29 @@
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="12">
+      <c r="C2" s="12"/>
+      <c r="D2" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="15">
         <v>45803.6277777778</v>
       </c>
-      <c r="E2" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="12">
+      <c r="J2" s="15">
         <v>45811.7541666667</v>
       </c>
-      <c r="K2" s="30">
+      <c r="K2" s="33">
         <v>45805.4909722222</v>
       </c>
     </row>
@@ -1831,27 +1843,27 @@
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="12">
+      <c r="B3" s="11"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="15">
         <v>45805.4243055556</v>
       </c>
-      <c r="E3" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="12">
+      <c r="J3" s="15">
         <v>45805.4458333333</v>
       </c>
     </row>
@@ -1859,27 +1871,27 @@
       <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="12">
+      <c r="B4" s="11"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="15">
         <v>45805.4513888889</v>
       </c>
-      <c r="E4" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="12">
+      <c r="I4" s="15">
         <v>45805.4590277778</v>
       </c>
-      <c r="J4" s="12">
+      <c r="J4" s="15">
         <v>45805.5020833333</v>
       </c>
     </row>
@@ -1887,27 +1899,27 @@
       <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="12">
+      <c r="B5" s="11"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="15">
         <v>45804.6597222222</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="12">
+      <c r="I5" s="15">
         <v>45805.4805555556</v>
       </c>
-      <c r="J5" s="12">
+      <c r="J5" s="15">
         <v>45805.4819444444</v>
       </c>
     </row>
@@ -1915,27 +1927,27 @@
       <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="12">
+      <c r="B6" s="11"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="15">
         <v>45805.6243055556</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6" s="12">
+      <c r="I6" s="15">
         <v>45805.6291666667</v>
       </c>
-      <c r="J6" s="12">
+      <c r="J6" s="15">
         <v>45805.6465277778</v>
       </c>
     </row>
@@ -1943,42 +1955,42 @@
       <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="19">
+      <c r="B7" s="11"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="21"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="23">
         <v>45803.7618055556</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="21"/>
-      <c r="H7" s="22"/>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="12">
+      <c r="B8" s="11"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="15">
         <v>45800.6409722222</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="K8" s="8" t="s">
+      <c r="K8" s="9" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1986,43 +1998,43 @@
       <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="12">
+      <c r="B9" s="11"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="15">
         <v>45803.6479166667</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="12">
+      <c r="C10" s="16"/>
+      <c r="D10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="26"/>
+      <c r="H10" s="15">
         <v>45806.3958333333</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G10" s="25"/>
-      <c r="K10" s="8" t="s">
+      <c r="K10" s="9" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2030,127 +2042,127 @@
       <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="12">
+      <c r="B11" s="25"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" s="15">
         <v>45800.7673611111</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="K11" s="30">
+      <c r="K11" s="33">
         <v>45806.4166666667</v>
       </c>
     </row>
     <row r="12" spans="2:9">
-      <c r="B12" s="24"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="12">
+      <c r="B12" s="25"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="15">
         <v>45800.7708333333</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I12" s="12"/>
+      <c r="I12" s="15"/>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="4">
         <v>11</v>
       </c>
-      <c r="B13" s="24"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="12">
+      <c r="B13" s="25"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" s="15">
         <v>45806.4916666667</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="I13" s="12">
+      <c r="I13" s="15">
         <v>45806.5027777778</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:8">
       <c r="A14" s="4">
         <v>12</v>
       </c>
-      <c r="B14" s="24"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="12">
+      <c r="B14" s="25"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H14" s="15">
         <v>45806.6125</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="4">
         <v>13</v>
       </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="12">
+      <c r="B15" s="25"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H15" s="15">
         <v>45806.7409722222</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="4">
         <v>14</v>
       </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="12">
+      <c r="B16" s="25"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="H16" s="15">
         <v>45806.3958333333</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="G16" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>57</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>58</v>
@@ -2158,7 +2170,7 @@
       <c r="J16" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="K16" s="8" t="s">
+      <c r="K16" s="9" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2166,30 +2178,30 @@
       <c r="A17" s="4">
         <v>15</v>
       </c>
-      <c r="B17" s="24"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="12">
+      <c r="B17" s="25"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="H17" s="15">
         <v>45806.5784722222</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="I17" s="12">
+      <c r="I17" s="15">
         <v>45806.5923611111</v>
       </c>
       <c r="J17" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="K17" s="8" t="s">
+      <c r="K17" s="9" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2197,24 +2209,24 @@
       <c r="A18" s="4">
         <v>16</v>
       </c>
-      <c r="B18" s="24"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="12">
+      <c r="B18" s="25"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H18" s="15">
         <v>45806.6388888889</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="I18" s="12">
+      <c r="I18" s="15">
         <v>45806.7541666667</v>
       </c>
     </row>
@@ -2222,76 +2234,76 @@
       <c r="A19" s="4">
         <v>17</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C19" s="23"/>
-      <c r="D19" s="12">
+      <c r="C19" s="24"/>
+      <c r="D19" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F19" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H19" s="15">
         <v>45807.3784722222</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F19" t="s">
-        <v>70</v>
-      </c>
-      <c r="G19" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="I19" s="12">
+      <c r="I19" s="15">
         <v>45807.4208333333</v>
       </c>
-      <c r="K19" s="8" t="s">
+      <c r="K19" s="9" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:8">
       <c r="A20" s="4">
         <v>18</v>
       </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="12">
+      <c r="B20" s="11"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F20" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="H20" s="15">
         <v>45807.4180555556</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="G20" s="27" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="4">
         <v>19</v>
       </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="12">
+      <c r="B21" s="11"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="H21" s="15">
         <v>45807.4486111111</v>
       </c>
-      <c r="E21" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="I21" s="12">
+      <c r="I21" s="15">
         <v>45807.6208333333</v>
       </c>
-      <c r="J21" s="12">
+      <c r="J21" s="15">
         <v>45811.5145833333</v>
       </c>
     </row>
@@ -2299,53 +2311,53 @@
       <c r="A22" s="4">
         <v>19</v>
       </c>
-      <c r="B22" s="10"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="12">
+      <c r="B22" s="11"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="H22" s="15">
         <v>45807.4791666667</v>
       </c>
-      <c r="E22" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="H22" s="7" t="s">
-        <v>83</v>
-      </c>
       <c r="I22" s="4"/>
-      <c r="J22" s="12">
+      <c r="J22" s="15">
         <v>45811.4722222222</v>
       </c>
-      <c r="K22" s="8"/>
+      <c r="K22" s="9"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="4">
         <v>21</v>
       </c>
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="12">
+      <c r="C23" s="12"/>
+      <c r="D23" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F23" t="s">
+        <v>86</v>
+      </c>
+      <c r="G23" t="s">
+        <v>87</v>
+      </c>
+      <c r="H23" s="15">
         <v>45811.3958333333</v>
       </c>
-      <c r="E23" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="G23" t="s">
-        <v>86</v>
-      </c>
-      <c r="H23" t="s">
-        <v>87</v>
-      </c>
-      <c r="I23" s="12">
+      <c r="I23" s="15">
         <v>45811.4368055556</v>
       </c>
     </row>
@@ -2353,27 +2365,27 @@
       <c r="A24" s="4">
         <v>22</v>
       </c>
-      <c r="B24" s="24"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="12">
+      <c r="B24" s="25"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E24" t="s">
+        <v>89</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H24" s="15">
         <v>45811.4979166667</v>
       </c>
-      <c r="E24" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="F24" t="s">
-        <v>89</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="H24" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="I24" s="12">
+      <c r="I24" s="15">
         <v>45811.5</v>
       </c>
-      <c r="J24" s="12">
+      <c r="J24" s="15">
         <v>45811.5104166667</v>
       </c>
     </row>
@@ -2381,24 +2393,24 @@
       <c r="A25" s="4">
         <v>23</v>
       </c>
-      <c r="B25" s="24"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="12">
+      <c r="B25" s="25"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="H25" s="15">
         <v>45811.4180555556</v>
       </c>
-      <c r="E25" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="H25" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="J25" s="12">
+      <c r="J25" s="15">
         <v>45811.6520833333</v>
       </c>
     </row>
@@ -2406,24 +2418,24 @@
       <c r="A26" s="4">
         <v>24</v>
       </c>
-      <c r="B26" s="24"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="12">
+      <c r="B26" s="25"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="H26" s="15">
         <v>45811.3854166667</v>
       </c>
-      <c r="E26" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="H26" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="I26" s="12">
+      <c r="I26" s="15">
         <v>45811.6583333333</v>
       </c>
     </row>
@@ -2431,27 +2443,27 @@
       <c r="A27" s="4">
         <v>25</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="28">
+      <c r="B27" s="25"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="H27" s="29">
         <v>0.661111111111111</v>
       </c>
-      <c r="E27" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="H27" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="I27" s="12">
+      <c r="I27" s="15">
         <v>45811.6875</v>
       </c>
-      <c r="J27" s="12">
+      <c r="J27" s="15">
         <v>45811.7201388889</v>
       </c>
     </row>
@@ -2459,56 +2471,66 @@
       <c r="A28" s="4">
         <v>26</v>
       </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="28">
+      <c r="B28" s="25"/>
+      <c r="C28" s="12"/>
+      <c r="E28" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="H28" s="29">
         <v>0.722916666666667</v>
       </c>
-      <c r="F28" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="H28" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="I28" s="28">
+      <c r="I28" s="29">
         <v>0.768055555555556</v>
       </c>
     </row>
-    <row r="29" s="3" customFormat="1" spans="1:1">
-      <c r="A29" s="29" t="s">
+    <row r="29" s="3" customFormat="1" spans="1:11">
+      <c r="A29" s="30" t="s">
         <v>105</v>
       </c>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
+      <c r="K29" s="31"/>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="4">
         <v>27</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="11" t="s">
         <v>106</v>
       </c>
       <c r="C30" s="4"/>
-      <c r="D30" s="12">
+      <c r="D30" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="H30" s="15">
         <v>45828.8666666667</v>
       </c>
-      <c r="E30" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="H30" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="I30" s="12">
+      <c r="I30" s="15">
         <v>45831.5798611111</v>
       </c>
-      <c r="J30" s="12">
+      <c r="J30" s="15">
         <v>45831.6229166667</v>
       </c>
     </row>
@@ -2516,27 +2538,27 @@
       <c r="A31" s="4">
         <v>28</v>
       </c>
-      <c r="B31" s="10"/>
+      <c r="B31" s="11"/>
       <c r="C31" s="4"/>
-      <c r="D31" s="12">
+      <c r="D31" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="H31" s="15">
         <v>45831.6020833333</v>
       </c>
-      <c r="E31" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="H31" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="I31" s="12">
+      <c r="I31" s="15">
         <v>45831.7576388889</v>
       </c>
-      <c r="J31" s="12">
+      <c r="J31" s="15">
         <v>45831.7611111111</v>
       </c>
     </row>
@@ -2544,48 +2566,48 @@
       <c r="A32" s="4">
         <v>29</v>
       </c>
-      <c r="B32" s="10"/>
+      <c r="B32" s="11"/>
       <c r="C32" s="4"/>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="4">
         <v>30</v>
       </c>
-      <c r="B33" s="10"/>
+      <c r="B33" s="11"/>
       <c r="C33" s="4"/>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="4">
         <v>31</v>
       </c>
-      <c r="B34" s="10"/>
+      <c r="B34" s="11"/>
       <c r="C34" s="4"/>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="4">
         <v>32</v>
       </c>
-      <c r="B35" s="10"/>
+      <c r="B35" s="11"/>
       <c r="C35" s="4"/>
-      <c r="D35" s="12">
+      <c r="D35" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E35" t="s">
+        <v>115</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="H35" s="15">
         <v>45825.4013888889</v>
       </c>
-      <c r="E35" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="F35" t="s">
-        <v>115</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="H35" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="I35" s="12">
+      <c r="I35" s="15">
         <v>45825.4069444444</v>
       </c>
-      <c r="J35" s="12">
+      <c r="J35" s="15">
         <v>45825.4395833333</v>
       </c>
     </row>
@@ -2593,49 +2615,49 @@
       <c r="A36" s="4">
         <v>33</v>
       </c>
-      <c r="B36" s="10"/>
+      <c r="B36" s="11"/>
       <c r="C36" s="4"/>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="4">
         <v>34</v>
       </c>
-      <c r="B37" s="10"/>
+      <c r="B37" s="11"/>
       <c r="C37" s="4"/>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="4">
         <v>35</v>
       </c>
-      <c r="B38" s="10"/>
+      <c r="B38" s="11"/>
       <c r="C38" s="4"/>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="4">
         <v>36</v>
       </c>
-      <c r="B39" s="10"/>
+      <c r="B39" s="11"/>
       <c r="C39" s="4"/>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="4">
         <v>37</v>
       </c>
-      <c r="B40" s="10"/>
+      <c r="B40" s="11"/>
       <c r="C40" s="4"/>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="4">
         <v>38</v>
       </c>
-      <c r="B41" s="10"/>
+      <c r="B41" s="11"/>
       <c r="C41" s="4"/>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="4">
         <v>39</v>
       </c>
-      <c r="B42" s="10"/>
+      <c r="B42" s="11"/>
       <c r="C42" s="4"/>
     </row>
     <row r="43" spans="1:3">
@@ -2664,17 +2686,17 @@
         <v>43</v>
       </c>
       <c r="B46" s="4"/>
-      <c r="C46" s="15"/>
-      <c r="D46" s="12">
+      <c r="C46" s="16"/>
+      <c r="D46" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E46" t="s">
+        <v>119</v>
+      </c>
+      <c r="H46" s="15">
         <v>45828.6854166667</v>
       </c>
-      <c r="E46" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F46" t="s">
-        <v>119</v>
-      </c>
-      <c r="K46" s="8" t="s">
+      <c r="K46" s="9" t="s">
         <v>120</v>
       </c>
     </row>
@@ -2683,29 +2705,34 @@
         <v>44</v>
       </c>
       <c r="B47" s="4"/>
-      <c r="C47" s="15"/>
-      <c r="D47" s="12">
+      <c r="C47" s="16"/>
+      <c r="D47" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E47" t="s">
+        <v>122</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="H47" s="15">
         <v>45830.6027777778</v>
       </c>
-      <c r="E47" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="F47" t="s">
-        <v>122</v>
-      </c>
-      <c r="G47" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="I47" s="12">
+      <c r="I47" s="15">
         <v>45830.6506944444</v>
       </c>
-      <c r="K47" s="8" t="s">
+      <c r="K47" s="9" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" s="4">
         <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="4:4">
+      <c r="D50" s="5" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>